<commit_message>
reevaluate regressions as polynomial, reorganize files
</commit_message>
<xml_diff>
--- a/Data/Taxa_Literature_Mining.xlsx
+++ b/Data/Taxa_Literature_Mining.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danielle Barnas\Documents\Repositories\Community_Functional_Diversity\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E90916-986C-4F93-B2DD-DB5735F7FD7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44F5AEF-F3BF-4AF4-9517-FAA2AF14E248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3732" yWindow="0" windowWidth="19320" windowHeight="10908" xr2:uid="{4E17320D-F6DB-46AC-844F-CBD89A61B4AE}"/>
+    <workbookView xWindow="9324" yWindow="6720" windowWidth="13836" windowHeight="7992" xr2:uid="{4E17320D-F6DB-46AC-844F-CBD89A61B4AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="116">
   <si>
     <t>Year</t>
   </si>
@@ -114,95 +114,6 @@
   </si>
   <si>
     <t>https://link.springer.com/article/10.1007/s00338-016-1425-0</t>
-  </si>
-  <si>
-    <t>Lithophyllum kotschyanum: growth, density for buoyant weights;  calcite density of 2.71 g cm−3 for L. kotschyanum, in accordance with the mineral form of CaCO3 deposited by each taxon. Rates of net calcification were normalized to the area of organisms estimated using wax dipping (Stimson and Kinzie 1991).</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Parameterization of the response of calcification to temperature and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="24"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>p</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="24"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CO</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="subscript"/>
-        <sz val="24"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="24"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> in the coral </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="24"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Acropora pulchra</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="24"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and the alga </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="24"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lithophyllum kotschyanum</t>
-    </r>
   </si>
   <si>
     <t>Comeau et al. (Pete and Bob)</t>
@@ -241,6 +152,429 @@
   </si>
   <si>
     <t>Calcification and size</t>
+  </si>
+  <si>
+    <t>https://besjournals.onlinelibrary.wiley.com/doi/full/10.1111/1365-2435.13358</t>
+  </si>
+  <si>
+    <t>Zawada et al.</t>
+  </si>
+  <si>
+    <t>Traits EcoFun</t>
+  </si>
+  <si>
+    <t>Morphological traits can track coral reef responses to the Anthropocene</t>
+  </si>
+  <si>
+    <t>connecting traits to ecological functioning</t>
+  </si>
+  <si>
+    <t>Feeding Trait</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/267923781_Feeding_ecology_of_intertidal_sea_anemones_Cnidaria_Actiniaria_food_sources_and_trophic_parameters#fullTextFileContent</t>
+  </si>
+  <si>
+    <t>Feeding ecology of intertidal sea anemones (Cnidaria, Actiniaria): food sources and trophic parameters</t>
+  </si>
+  <si>
+    <r>
+      <t>Acu</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ñ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a and Zamponi</t>
+    </r>
+  </si>
+  <si>
+    <t>Anemone;  polyphagous (preying on a wide variety of prey) and opportunistic (taking their prey as a function of each prey species' availability)</t>
+  </si>
+  <si>
+    <t>https://www.mdpi.com/2076-2615/12/10/1283</t>
+  </si>
+  <si>
+    <t>Zooxanthellate</t>
+  </si>
+  <si>
+    <t>Lendenfeldia symbiosis</t>
+  </si>
+  <si>
+    <t>Light Availability Affects the Symbiosis of Sponge Specific Cyanobacteria and the Common Blue Aquarium Sponge (Lendenfeldia chondrodes)</t>
+  </si>
+  <si>
+    <t>Curdt et al.</t>
+  </si>
+  <si>
+    <t>Avrainvilliea erecta; rapid growth (Smithet al. 2004), adaptability to low nutrient environments (Lobban and Harrison 1994, Smith etal. 2004, Malta et al. 2005)</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/328113865_A_new_record_of_Avrainvillea_cf_erecta_Berkeley_A_Gepp_E_S_Gepp_Bryopsidales_Chlorophyta_from_urbanized_estuaries_in_the_Hawaiian_Islands#fullTextFileContent</t>
+  </si>
+  <si>
+    <t>A new record of Avrainvillea cf. erecta (Berkeley) A. Gepp &amp; E. S. Gepp (Bryopsidales, Chlorophyta) from urbanized estuaries in the Hawaiian Islands</t>
+  </si>
+  <si>
+    <t>Nutrient uptake</t>
+  </si>
+  <si>
+    <t>https://scholarspace.manoa.hawaii.edu/items/34ae25b7-fbff-4f21-8490-b2c2051bf049</t>
+  </si>
+  <si>
+    <t>A Growing Problem: The Missing Link for Ecological Success by the Invasive Avrainvillea</t>
+  </si>
+  <si>
+    <t>Albright and Smith</t>
+  </si>
+  <si>
+    <t>Peyton</t>
+  </si>
+  <si>
+    <t>Wade et al</t>
+  </si>
+  <si>
+    <t>Aquatic invasive species impacts in Hawaiian soft sediment habitats, Ph.D. University of Hawaiʻi at Mānoa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avrainvilliea erecta; perennial, the adult forms can live for long periods. Although it is a slow growing plant, as a perennial, it can outlive other more short-lived species, giving Avrainvillea an additional advantage over native species (Peyton 2009). </t>
+  </si>
+  <si>
+    <t>Life Span and growth</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Parameterization of the response of calcification to temperature and </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CO</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> in the coral </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Acropora pulchra</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and the alga </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lithophyllum kotschyanum</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.frontiersin.org/articles/10.3389/fmars.2019.00402/full</t>
+  </si>
+  <si>
+    <t>Avrainvilliea sp; invasive in hawaii, resilient to light and nutrient loading</t>
+  </si>
+  <si>
+    <t>Veazey et al.</t>
+  </si>
+  <si>
+    <t>Ecological role</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Present-Day Distribution and Potential Spread of the Invasive Green Alga </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Avrainvillea amadelpha</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Around the Main Hawaiian Islands</t>
+    </r>
+  </si>
+  <si>
+    <t>Avrainvilliea erecta; growth in groundwater, high nutrients; As a perennial, the adult forms can live for long periods. ; Although it is a slow growing plant, as a perennial, it can outlive other more short-lived species, giving Avrainvillea an additional advantage over native species (Peyton 2009). ; Over 23 of 54 acres were successfully cleared by hand by volunteers in 7,000 man hours (“The Great Huki Project”). In less than six years, the algae have grown back and covers the area once more (Figure 2.5).</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
+  <si>
+    <t>https://link.springer.com/article/10.1007/BF02395280</t>
+  </si>
+  <si>
+    <t>Halimeda biomass, growth rates and sediment generation on reefs in the central great barrier reef province</t>
+  </si>
+  <si>
+    <t>Drew</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Halimeda; Biomass doubling time of 15 d and production of 6.9 g dry wt m−2 d−1 are considerably higher than previously reported values forHalimeda vegetation </t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/abs/10.1111/maec.12371</t>
+  </si>
+  <si>
+    <t>Growth rates and ecology of coralline rhodoliths from the Ras Ghamila back reef lagoon, Red Sea</t>
+  </si>
+  <si>
+    <t>Caragnano et al.</t>
+  </si>
+  <si>
+    <t>CCA growth rate (fruticose morphology); The highest accretion rate and common presence of L. kotschyanum indicate its importance as carbonate producer in tropical reef.</t>
+  </si>
+  <si>
+    <t>Lithophyllum kotschyanum: density for buoyant weights;  calcite density of 2.71 g cm−3 for L. kotschyanum, in accordance with the mineral form of CaCO3 deposited by each taxon. Rates of net calcification were normalized to the area of organisms estimated using wax dipping (Stimson and Kinzie 1991).</t>
+  </si>
+  <si>
+    <t>Bezy et al.</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/288004373_Contrasting_Psammocora-dominated_coral_communities_in_Costa_Rica_tropical_eastern_Pacific</t>
+  </si>
+  <si>
+    <t>Constrasting Psammocora-dominated coral communities in Costa Rica, tropical eastern Pacific</t>
+  </si>
+  <si>
+    <t>Dinesen</t>
+  </si>
+  <si>
+    <t>Shade-dwelling corals of the Great Barrier Reef.</t>
+  </si>
+  <si>
+    <t>https://www.int-res.com/articles/meps/10/m010p173.pdf</t>
+  </si>
+  <si>
+    <t>Shade-preferring shade-tolerating corals (stylocoeniella armata, goniastrea stelligera, pavona chiriquiensis, leptoseris mycetoseroides, Cyphastrea microphthalma)</t>
+  </si>
+  <si>
+    <t>Growth of seven species of scleractinian corals in an upwelling environment of the eastern Pacific (Golfo de Papagayo, Costa Rica)</t>
+  </si>
+  <si>
+    <t>https://www.ingentaconnect.com/content/umrsmas/bullmar/2003/00000072/00000001/art00013</t>
+  </si>
+  <si>
+    <t>Jimenez and Cortez</t>
+  </si>
+  <si>
+    <t>Growth rate of P. acuta</t>
+  </si>
+  <si>
+    <t>Smith et al.</t>
+  </si>
+  <si>
+    <t>https://aslopubs.onlinelibrary.wiley.com/doi/abs/10.4319/lo.2004.49.6.1923</t>
+  </si>
+  <si>
+    <t>Halimeda spp growth</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Nutrient and growth dynamics of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Halimeda tuna</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> on Conch Reef, Florida Keys: Possible influence of internal tides on nutrient status and physiology</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/339564974_Dynamics_of_carbonate_sediment_production_by_Halimeda_implications_for_reef_carbonate_budgets</t>
+  </si>
+  <si>
+    <t>Dynamics of carbonate sediment production by Halimeda: implications for reef carbonate budgets</t>
+  </si>
+  <si>
+    <t>Sanguino et al.</t>
+  </si>
+  <si>
+    <t>Halimeda carbonate budget on coral reef</t>
+  </si>
+  <si>
+    <t>Toste et al.</t>
+  </si>
+  <si>
+    <t>Hydroclathrus clathratus</t>
+  </si>
+  <si>
+    <t>https://repositorio.uac.pt/handle/10400.3/2027</t>
+  </si>
+  <si>
+    <t>Life history and phenology of Hydroclathrus clathratus (Scytosiphonaceae, Phaeophyceae) in the Azores.</t>
+  </si>
+  <si>
+    <t>Correlated studies on season changes in the sexuality, growth rate, and longevity of complanate scytosiphon (Scytosiphonaceae: Phaeophyta) from southern Australia growing in situ</t>
+  </si>
+  <si>
+    <t>https://reader.elsevier.com/reader/sd/pii/0022098181901556?token=36237229FB4DA5F863A2B7E2A2CA03C3E9DD3A41A3D3BAAF56D1F214933B2FCA8B2FB4E431932879E9E7644217400C59&amp;originRegion=us-east-1&amp;originCreation=20230307010649</t>
+  </si>
+  <si>
+    <t>Clayton</t>
+  </si>
+  <si>
+    <t>Growth rate</t>
+  </si>
+  <si>
+    <t>Life span</t>
+  </si>
+  <si>
+    <t>Hydroclathrus clathratus; Scytophon plants had a lifespan of up to 12 or 13 wk, although they were often shorter lived.</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/pdf/10.1111/pre.12478</t>
+  </si>
+  <si>
+    <t>Hypnea pannosa</t>
+  </si>
+  <si>
+    <t>Nauer et al.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Thermal tolerance of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Hypnea pseudomusciformis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ecotypes (Cystocloniaceae, Rhodophyta) related to different floristic provinces along the Brazilian coast</t>
+    </r>
+  </si>
+  <si>
+    <t>Gracilaria verrucosa</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/251502774_Raft_culture_of_Gracilaria_edulis_in_open_sea_along_the_south-eastern_coast_of_India</t>
+  </si>
+  <si>
+    <t>Raft culture of Gracilaria edulis in open sea along the south-eastern coast of India</t>
+  </si>
+  <si>
+    <t>Meenakshisundaram et al.</t>
+  </si>
+  <si>
+    <t>Population Dynamics and Ecological Impacts of the Alien Macroalgae Galaxaura Rugosa (J.Ellis &amp; Solander) J.V.Lamouroux on the Israeli Shore</t>
+  </si>
+  <si>
+    <t>https://www.proquest.com/openview/1ff37cfa2469cbe11f1e9c01e4c0f82f/1?pq-origsite=gscholar&amp;cbl=2026366&amp;diss=y</t>
+  </si>
+  <si>
+    <t>Galaxaura rugosa</t>
+  </si>
+  <si>
+    <t>Ellis and Solander</t>
   </si>
 </sst>
 </file>
@@ -265,36 +599,33 @@
     </font>
     <font>
       <b/>
-      <sz val="24"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <i/>
-      <sz val="24"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <vertAlign val="subscript"/>
-      <sz val="24"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -317,20 +648,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -646,161 +985,703 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F108D8-B9C2-4010-AF28-74BCEE489640}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.109375" style="5" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="38" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" customWidth="1"/>
-    <col min="6" max="6" width="40.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="38" style="6" customWidth="1"/>
+    <col min="5" max="5" width="40.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="88" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="2">
         <v>2018</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>2017</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="2">
         <v>2018</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="2">
         <v>2005</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="36" x14ac:dyDescent="0.8">
+    </row>
+    <row r="6" spans="1:6" ht="58.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="4">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2">
         <v>2016</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="D6" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2">
+        <v>2013</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="4">
-        <v>2013</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>29</v>
-      </c>
+      <c r="F8" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1995</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2018</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="2">
+        <v>2009</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2019</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1983</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" s="2">
+        <v>2016</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2006</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1983</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2003</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="2">
+        <v>2004</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2003</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1981</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2022</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B25" s="2">
+        <v>2011</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D25" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="2">
+        <v>2015</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F40" s="6"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F42" s="6"/>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F52" s="6"/>
+    </row>
+    <row r="53" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F53" s="6"/>
+    </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F54" s="6"/>
+    </row>
+    <row r="55" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F55" s="6"/>
+    </row>
+    <row r="56" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F56" s="6"/>
+    </row>
+    <row r="57" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F57" s="6"/>
+    </row>
+    <row r="58" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F58" s="6"/>
+    </row>
+    <row r="59" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F59" s="6"/>
+    </row>
+    <row r="60" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F60" s="6"/>
+    </row>
+    <row r="61" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F61" s="6"/>
+    </row>
+    <row r="62" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F62" s="6"/>
+    </row>
+    <row r="63" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F63" s="6"/>
+    </row>
+    <row r="64" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F64" s="6"/>
+    </row>
+    <row r="65" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F66" s="6"/>
+    </row>
+    <row r="67" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F68" s="6"/>
+    </row>
+    <row r="69" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F69" s="6"/>
+    </row>
+    <row r="70" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F70" s="6"/>
+    </row>
+    <row r="71" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F71" s="6"/>
+    </row>
+    <row r="72" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F72" s="6"/>
+    </row>
+    <row r="73" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F73" s="6"/>
+    </row>
+    <row r="74" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F74" s="6"/>
+    </row>
+    <row r="75" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F75" s="6"/>
+    </row>
+    <row r="76" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F76" s="6"/>
+    </row>
+    <row r="77" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F77" s="6"/>
+    </row>
+    <row r="78" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F78" s="6"/>
+    </row>
+    <row r="79" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F79" s="6"/>
+    </row>
+    <row r="80" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F80" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D18" r:id="rId1" display="https://www.int-res.com/articles/meps/10/m010p173.pdf" xr:uid="{0E294619-51ED-46CD-851C-42F8ED49EF64}"/>
+    <hyperlink ref="E20" r:id="rId2" xr:uid="{28AEEA49-E38E-460A-ABC1-843A1461C745}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add moorea biocode info for species ID
</commit_message>
<xml_diff>
--- a/Data/Taxa_Literature_Mining.xlsx
+++ b/Data/Taxa_Literature_Mining.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danielle Barnas\Documents\Repositories\Community_Functional_Diversity\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44F5AEF-F3BF-4AF4-9517-FAA2AF14E248}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B46FBA-82A7-4357-A7EC-CADC9EB619D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9324" yWindow="6720" windowWidth="13836" windowHeight="7992" xr2:uid="{4E17320D-F6DB-46AC-844F-CBD89A61B4AE}"/>
+    <workbookView xWindow="-38320" yWindow="-11940" windowWidth="18140" windowHeight="20350" xr2:uid="{4E17320D-F6DB-46AC-844F-CBD89A61B4AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$26</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="181">
   <si>
     <t>Year</t>
   </si>
@@ -576,12 +579,232 @@
   <si>
     <t>Ellis and Solander</t>
   </si>
+  <si>
+    <t>Differential growth responses to water flow and reduced pH in tropical marine macroalgae</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0022098117301636?casa_token=hXGhcdamkkIAAAAA:BmNjmmvhUUzmrU6rVeS5c_-HUsAn6RXtj4igkRPz3lMU8TPsVlyk2yD8Jc61CshOCQQqulKr</t>
+  </si>
+  <si>
+    <t>Ho and Carpenter</t>
+  </si>
+  <si>
+    <t>Growth and Calcification and Methods</t>
+  </si>
+  <si>
+    <t>Moorea: Dictyota bartayresiana, Lobophora variegata, Amansia rhodantha (non-calcifying); methods: using clear nylon monofilament mesh bag to envelop algae</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/abs/10.1111/jpy.13158</t>
+  </si>
+  <si>
+    <t>Amphiroa fragilissima calcification</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Transcriptomic and Physiological Responses of the Tropical Reef Calcified Macroalga </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Amphiroa fragilissima</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="24"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to Elevated Temperature</t>
+    </r>
+  </si>
+  <si>
+    <t>Yang et al.</t>
+  </si>
+  <si>
+    <t>Calcification</t>
+  </si>
+  <si>
+    <t>https://repository.naturalis.nl/pub/525876/BLUM1989034001015.pdf</t>
+  </si>
+  <si>
+    <t>Seaweeds of the Snellius-II Expedition. Chlorophyta: Caulerpales (except Caulerpa and Halimeda)</t>
+  </si>
+  <si>
+    <t>Coppejans and Prud'homme van Reine</t>
+  </si>
+  <si>
+    <t>Avrainvillea erecta calcification</t>
+  </si>
+  <si>
+    <t>Paul and Hay</t>
+  </si>
+  <si>
+    <t>Seaweed susceptibility to herbivory: chemical and morphological correlates</t>
+  </si>
+  <si>
+    <t>https://www.jstor.org/stable/24825450</t>
+  </si>
+  <si>
+    <t>Caulerpa spp.</t>
+  </si>
+  <si>
+    <t>Ecological role and Morphology</t>
+  </si>
+  <si>
+    <t>Dictyosphaeria cavernosa nitrogen limitation</t>
+  </si>
+  <si>
+    <t>Larned and Simson</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/235938802_Nitrogen-limited_growth_in_the_coral_reef_chlorophyte_Dictyosphaeria_cavernosa_and_the_effect_of_exposure_to_sediment-derived_nitrogen_on_growth</t>
+  </si>
+  <si>
+    <t>Nitrogen-limited growth in the coral reef chlorophyte Dictyosphaeria cavernosa, and the effect of exposure to sediment-derived nitrogen on growth</t>
+  </si>
+  <si>
+    <t>https://zslpublications.onlinelibrary.wiley.com/doi/full/10.1002/rse2.355</t>
+  </si>
+  <si>
+    <t>benthic communities: calcification: cyanobacteria, dictyosphaeria, lobophora</t>
+  </si>
+  <si>
+    <t>Recurring bleaching events disrupt the spatial properties of coral reef benthic communities across scales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ford et al. </t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/abs/10.2216/i0031-8884-38-3-184.1</t>
+  </si>
+  <si>
+    <t>Morphology</t>
+  </si>
+  <si>
+    <t>Clerck and Coppejans</t>
+  </si>
+  <si>
+    <t>Two new species of Dictyota (Dictyotales, Phaeophyta) from the Indo-Malayan region</t>
+  </si>
+  <si>
+    <t>dictyota friabilis morphology and characteristics</t>
+  </si>
+  <si>
+    <t>Gracilaria verrucosa, non calcified</t>
+  </si>
+  <si>
+    <t>Dawes</t>
+  </si>
+  <si>
+    <t>Seasonal Proximate Constituents and Caloric Values in Seagrasses and Algae on the West Coast of Florida</t>
+  </si>
+  <si>
+    <t>https://www.jstor.org/stable/4297124?casa_token=fBB3BwDWP5AAAAAA%3AZBCy9w9MTem1H9LHuMEGx61AHRBEI_CRtzu7NXWrSZ-PBW_cYzVCmaIj_Txxv1roVWDvrIPFOvDZSiMDCyQaNzeE3jouUaCTQZWOtLVrobmYjy9cHQ</t>
+  </si>
+  <si>
+    <t>Sponge distribution and the presence of photosymbionts in Moorea, French Polynesia</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/298806734_Sponge_distribution_and_the_presence_of_photosymbionts_in_Moorea_French_Polynesia</t>
+  </si>
+  <si>
+    <t>Sponges of Moorea</t>
+  </si>
+  <si>
+    <t>Freeman and Easson</t>
+  </si>
+  <si>
+    <t>https://onlinelibrary.wiley.com/doi/abs/10.1111/maec.12298</t>
+  </si>
+  <si>
+    <t>Padina boryana identification in Moorea</t>
+  </si>
+  <si>
+    <t>Fong et al.</t>
+  </si>
+  <si>
+    <t>Size matters: experimental partitioning of the strength of fish herbivory on a fringing coral reef in Moorea, French Polynesia</t>
+  </si>
+  <si>
+    <t>https://sci-hubtw.hkvisa.net/10.1146/annurev.es.17.110186.001421</t>
+  </si>
+  <si>
+    <t>Crustose corallines Ecology and morphology</t>
+  </si>
+  <si>
+    <t>Ecology and Morphology</t>
+  </si>
+  <si>
+    <t>Steneck</t>
+  </si>
+  <si>
+    <t>The ecology of coralline algal crusts: convergent patterns and adapative strategies</t>
+  </si>
+  <si>
+    <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC5539699/</t>
+  </si>
+  <si>
+    <t>Cyphastrea microphthalma morphology</t>
+  </si>
+  <si>
+    <t>Cyphastrea salae, a new species of hard coral from Lord Howe Island, Australia (Scleractinia, Merulinidae)</t>
+  </si>
+  <si>
+    <t>Baird et al.</t>
+  </si>
+  <si>
+    <t>https://www.frontiersin.org/articles/10.3389/fmars.2020.00128/full?&amp;utm_source=Email_to_authors_&amp;utm_medium=Email&amp;utm_content=T1_11.5e1_author&amp;utm_campaign=Email_publication&amp;field=&amp;journalName=Frontiers_in_Marine_Science&amp;id=498911</t>
+  </si>
+  <si>
+    <t>Danafungia scruposa morphology</t>
+  </si>
+  <si>
+    <t>Passive and active removal of marine microplastics by a mushroom coral (Danafungia scruposa)</t>
+  </si>
+  <si>
+    <t>Corona et al.</t>
+  </si>
+  <si>
+    <t>https://www.indopacificimages.com/wp-content/uploads/2013/07/TNC_REA_Raja-Ampat_2003.pdf#page=63</t>
+  </si>
+  <si>
+    <t>Montipora grisea encrusting growth form</t>
+  </si>
+  <si>
+    <t>Coral diversity and the status of coral reefs in the Raja Ampat Islands</t>
+  </si>
+  <si>
+    <t>Turak and Souhoka</t>
+  </si>
+  <si>
+    <t>https://citeseerx.ist.psu.edu/document?repid=rep1&amp;type=pdf&amp;doi=217e959cb164bed67ae3dd612ac38aadb781d1de</t>
+  </si>
+  <si>
+    <t>New species described in Corals of the World</t>
+  </si>
+  <si>
+    <t>Veron</t>
+  </si>
+  <si>
+    <t>Montipora setos growth form, described as having small branches or encrusting with compact branches or irregular upgrowths (book)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -605,13 +828,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -627,13 +843,44 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -645,10 +892,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -668,11 +916,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -985,10 +1240,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4F108D8-B9C2-4010-AF28-74BCEE489640}">
-  <dimension ref="A1:F80"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -998,11 +1254,12 @@
     <col min="3" max="3" width="15.21875" style="2" customWidth="1"/>
     <col min="4" max="4" width="38" style="6" customWidth="1"/>
     <col min="5" max="5" width="40.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="88" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="3.109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="88" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1018,11 +1275,12 @@
       <c r="E1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>8</v>
       </c>
@@ -1038,11 +1296,12 @@
       <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="1"/>
+      <c r="G2" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1058,11 +1317,11 @@
       <c r="E3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="G3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -1078,11 +1337,11 @@
       <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="G4" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1098,11 +1357,11 @@
       <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="G5" s="6" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="58.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="58.8" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>26</v>
       </c>
@@ -1118,11 +1377,11 @@
       <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
@@ -1135,11 +1394,11 @@
       <c r="D7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="G7" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>32</v>
       </c>
@@ -1152,14 +1411,14 @@
       <c r="D8" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="G8" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>39</v>
       </c>
@@ -1175,11 +1434,11 @@
       <c r="E9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="G9" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>45</v>
       </c>
@@ -1195,11 +1454,11 @@
       <c r="E10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="G10" s="6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>54</v>
       </c>
@@ -1215,11 +1474,11 @@
       <c r="E11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="G11" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>52</v>
       </c>
@@ -1235,11 +1494,12 @@
       <c r="E12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="1"/>
+      <c r="G12" s="6" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>53</v>
       </c>
@@ -1252,11 +1512,12 @@
       <c r="D13" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F13" s="1"/>
+      <c r="G13" s="6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>61</v>
       </c>
@@ -1272,11 +1533,11 @@
       <c r="E14" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>68</v>
       </c>
@@ -1292,11 +1553,12 @@
       <c r="E15" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="1"/>
+      <c r="G15" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>72</v>
       </c>
@@ -1312,11 +1574,12 @@
       <c r="E16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="1"/>
+      <c r="G16" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>75</v>
       </c>
@@ -1332,9 +1595,10 @@
       <c r="E17" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F17" s="1"/>
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>78</v>
       </c>
@@ -1342,7 +1606,7 @@
         <v>1983</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>62</v>
+        <v>134</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>79</v>
@@ -1350,11 +1614,11 @@
       <c r="E18" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="G18" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>84</v>
       </c>
@@ -1370,11 +1634,12 @@
       <c r="E19" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="1"/>
+      <c r="G19" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>86</v>
       </c>
@@ -1390,11 +1655,12 @@
       <c r="E20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="F20" s="1"/>
+      <c r="G20" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>92</v>
       </c>
@@ -1410,11 +1676,11 @@
       <c r="E21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="G21" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>94</v>
       </c>
@@ -1430,11 +1696,12 @@
       <c r="E22" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F22" s="6" t="s">
+      <c r="F22" s="1"/>
+      <c r="G22" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>100</v>
       </c>
@@ -1450,11 +1717,12 @@
       <c r="E23" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="1"/>
+      <c r="G23" s="6" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>106</v>
       </c>
@@ -1464,17 +1732,18 @@
       <c r="C24" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F24" s="6" t="s">
+      <c r="F24" s="1"/>
+      <c r="G24" s="6" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>111</v>
       </c>
@@ -1490,11 +1759,12 @@
       <c r="E25" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F25" s="6" t="s">
+      <c r="F25" s="1"/>
+      <c r="G25" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>115</v>
       </c>
@@ -1510,178 +1780,448 @@
       <c r="E26" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F26" s="6" t="s">
+      <c r="F26" s="1"/>
+      <c r="G26" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F36" s="6"/>
-    </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F37" s="6"/>
-    </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F39" s="6"/>
-    </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F40" s="6"/>
-    </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F41" s="6"/>
-    </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F42" s="6"/>
-    </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F43" s="6"/>
-    </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F44" s="6"/>
-    </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F45" s="6"/>
-    </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F46" s="6"/>
-    </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F47" s="6"/>
-    </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F48" s="6"/>
-    </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F49" s="6"/>
-    </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F50" s="6"/>
-    </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F51" s="6"/>
-    </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F52" s="6"/>
-    </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F53" s="6"/>
-    </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F54" s="6"/>
-    </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F55" s="6"/>
-    </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F56" s="6"/>
-    </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F57" s="6"/>
-    </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F58" s="6"/>
-    </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F59" s="6"/>
-    </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F60" s="6"/>
-    </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F61" s="6"/>
-    </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F62" s="6"/>
-    </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F63" s="6"/>
-    </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F64" s="6"/>
-    </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F65" s="6"/>
-    </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F66" s="6"/>
-    </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F67" s="6"/>
-    </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F68" s="6"/>
-    </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F69" s="6"/>
-    </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F70" s="6"/>
-    </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F71" s="6"/>
-    </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F72" s="6"/>
-    </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F73" s="6"/>
-    </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F74" s="6"/>
-    </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F75" s="6"/>
-    </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F76" s="6"/>
-    </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F77" s="6"/>
-    </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F78" s="6"/>
-    </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F79" s="6"/>
-    </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F80" s="6"/>
+    <row r="27" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" t="s">
+        <v>116</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="A28" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2021</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1989</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" t="s">
+        <v>127</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1986</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1996</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2023</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1999</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1986</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2016</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2016</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1986</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2017</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2020</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B40" s="2">
+        <v>2003</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B41" s="2">
+        <v>2002</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G47" s="6"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G57" s="6"/>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G58" s="6"/>
+    </row>
+    <row r="59" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G60" s="6"/>
+    </row>
+    <row r="61" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G63" s="6"/>
+    </row>
+    <row r="64" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G64" s="6"/>
+    </row>
+    <row r="65" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G67" s="6"/>
+    </row>
+    <row r="68" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G68" s="6"/>
+    </row>
+    <row r="69" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G69" s="6"/>
+    </row>
+    <row r="70" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G70" s="6"/>
+    </row>
+    <row r="71" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G71" s="6"/>
+    </row>
+    <row r="72" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G72" s="6"/>
+    </row>
+    <row r="73" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G73" s="6"/>
+    </row>
+    <row r="74" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G74" s="6"/>
+    </row>
+    <row r="75" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G75" s="6"/>
+    </row>
+    <row r="76" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G76" s="6"/>
+    </row>
+    <row r="77" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G77" s="6"/>
+    </row>
+    <row r="78" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G78" s="6"/>
+    </row>
+    <row r="79" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G79" s="6"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G26" xr:uid="{A4F108D8-B9C2-4010-AF28-74BCEE489640}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Calcification and size"/>
+        <filter val="Ecological role"/>
+        <filter val="Feeding Trait"/>
+        <filter val="Identification"/>
+        <filter val="Traits"/>
+        <filter val="Traits EcoFun"/>
+        <filter val="Zooxanthellate"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <hyperlinks>
     <hyperlink ref="D18" r:id="rId1" display="https://www.int-res.com/articles/meps/10/m010p173.pdf" xr:uid="{0E294619-51ED-46CD-851C-42F8ED49EF64}"/>
     <hyperlink ref="E20" r:id="rId2" xr:uid="{28AEEA49-E38E-460A-ABC1-843A1461C745}"/>
+    <hyperlink ref="E8" r:id="rId3" xr:uid="{28C982EC-3C22-4F9C-9F37-695F24B1DE5C}"/>
+    <hyperlink ref="D29" r:id="rId4" display="https://repository.naturalis.nl/pub/525876/BLUM1989034001015.pdf" xr:uid="{4568F10B-96A4-4F28-817D-440B721FA691}"/>
+    <hyperlink ref="D40" r:id="rId5" location="page=63" display="https://www.indopacificimages.com/wp-content/uploads/2013/07/TNC_REA_Raja-Ampat_2003.pdf - page=63" xr:uid="{86F10F7D-599A-45AA-B731-D05138026F51}"/>
+    <hyperlink ref="D41" r:id="rId6" display="https://citeseerx.ist.psu.edu/document?repid=rep1&amp;type=pdf&amp;doi=217e959cb164bed67ae3dd612ac38aadb781d1de" xr:uid="{FDD4748F-5084-459C-B20E-E7E9C6399A12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>